<commit_message>
Feature: add arrows (arrow_n). Fixed bugs, removed unnecessary code.
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/xlsx/area-multiple.xlsx
+++ b/inst/extdata/examples/xlsx/area-multiple.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">tab</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t xml:space="preserve">3, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">style</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -423,7 +429,15 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -441,25 +455,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">

</xml_diff>